<commit_message>
Create excel graphs for data overview
</commit_message>
<xml_diff>
--- a/Results_HNSW/Results_HNSW.xlsx
+++ b/Results_HNSW/Results_HNSW.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Univer\3_kurs\Comparison_of_methods_for_multilingual_semantic_search\Results_HNSW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABA8B241-D49B-4CDC-81E9-9217EE4B7231}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D39DC73E-A699-4461-BAC3-134857B100ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{8E0A40BA-44C0-4AFD-9FBD-B7C4CB56C13F}"/>
   </bookViews>
@@ -512,7 +512,7 @@
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <selection activeCell="O22" sqref="O22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -524,6 +524,12 @@
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17" customWidth="1"/>
+    <col min="14" max="14" width="17.85546875" customWidth="1"/>
+    <col min="16" max="16" width="16.7109375" customWidth="1"/>
+    <col min="18" max="18" width="16.7109375" customWidth="1"/>
+    <col min="20" max="20" width="16.7109375" customWidth="1"/>
+    <col min="22" max="22" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -1172,8 +1178,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>